<commit_message>
Updating the Data Dictionary
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thezo\Desktop\intro-to-buisness\Data Stuff 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10C43495-E9CE-42BF-8B3C-351357B9189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4E44D5-6818-4493-A4FE-0E6D4B3C57B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="42">
   <si>
     <t>Members</t>
   </si>
@@ -106,6 +106,51 @@
   </si>
   <si>
     <t>Privilage_Level</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Item_ID</t>
+  </si>
+  <si>
+    <t>Item_Description</t>
+  </si>
+  <si>
+    <t>Item_Price</t>
+  </si>
+  <si>
+    <t>OnHand</t>
+  </si>
+  <si>
+    <t>numerical</t>
+  </si>
+  <si>
+    <t>Invoices</t>
+  </si>
+  <si>
+    <t>Invo_Num</t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Foreign key</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Total_Sale</t>
+  </si>
+  <si>
+    <t>num</t>
   </si>
 </sst>
 </file>
@@ -206,6 +251,36 @@
     <tableColumn id="4" xr3:uid="{F64E5F59-20B4-4E0F-B0E5-F967AABB64C9}" name="Max Field Size"/>
     <tableColumn id="5" xr3:uid="{3680EF33-EC9F-402C-B95B-FC925D181487}" name="Primary Key"/>
     <tableColumn id="14" xr3:uid="{023311DA-4134-45A9-8EC4-7F91D2D59F62}" name="Extra Info"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{406A4BB3-B232-4B67-AA7E-F264FDEBADFB}" name="Table134" displayName="Table134" ref="A28:F36" totalsRowShown="0">
+  <autoFilter ref="A28:F36" xr:uid="{406A4BB3-B232-4B67-AA7E-F264FDEBADFB}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B849715B-CC0C-4349-B8FA-3926E6966DC1}" name="Attribute Name"/>
+    <tableColumn id="2" xr3:uid="{1306795C-E226-43D8-A0D6-32BD621B0B1C}" name="Required"/>
+    <tableColumn id="3" xr3:uid="{8946C1C3-4C4A-46DF-BFE6-829F44BAA3E5}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{67815117-002A-4137-AC92-1965C360EA36}" name="Max Field Size"/>
+    <tableColumn id="5" xr3:uid="{9F636FFA-1797-49F4-A4FC-233AB9302427}" name="Primary Key"/>
+    <tableColumn id="14" xr3:uid="{9C8122BF-29BD-473C-8E15-5EEF2C97D095}" name="Extra Info"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6C1F0A51-76F6-4AA0-9857-5A2A4275CD95}" name="Table1345" displayName="Table1345" ref="A41:F49" totalsRowShown="0">
+  <autoFilter ref="A41:F49" xr:uid="{6C1F0A51-76F6-4AA0-9857-5A2A4275CD95}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{F43B26AF-6045-4F0D-BA6B-D12B542A9718}" name="Attribute Name"/>
+    <tableColumn id="2" xr3:uid="{22E89A70-19F7-4330-BE3E-FEE5BBD009C9}" name="Required"/>
+    <tableColumn id="3" xr3:uid="{FFFE5825-1643-467F-8338-A34544396C70}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{51AFC560-649E-4DAF-ADCE-FB3B786EEE9D}" name="Max Field Size"/>
+    <tableColumn id="5" xr3:uid="{7D0ADDE1-A7E1-4C86-BDF9-4523F04904D0}" name="Primary Key"/>
+    <tableColumn id="14" xr3:uid="{C56B1D60-9446-44A0-9774-C493981DBC20}" name="Extra Info"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -474,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -713,7 +788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -730,7 +805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -747,7 +822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -764,7 +839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -781,7 +856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -798,7 +873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -815,16 +890,236 @@
         <v>13</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="2">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46">
+        <v>12.2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A40:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>